<commit_message>
modified:   Engineering Yield Tracker (1).xlsx# modified:   app.py
</commit_message>
<xml_diff>
--- a/Engineering Yield Tracker (1).xlsx
+++ b/Engineering Yield Tracker (1).xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudadmwiwynn.sharepoint.com/teams/P2_Engineering1MasterFolder_Teams/Shared Documents/General/Engineering Section/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudadmwiwynn-my.sharepoint.com/personal/syahirah_sabudin_wiwynn_com/Documents/Documents/Umi/FPY-monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44224BDB-E454-4CB9-90B2-CC20DF41B10F}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B256F41-77E7-4439-8567-3F0F32F2D32B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="3" xr2:uid="{FA83E918-ED32-4BA0-A84E-C85110B79042}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12585" xr2:uid="{FA83E918-ED32-4BA0-A84E-C85110B79042}"/>
   </bookViews>
   <sheets>
-    <sheet name="MDA" sheetId="2" r:id="rId1"/>
-    <sheet name="ICT" sheetId="6" r:id="rId2"/>
-    <sheet name="BST" sheetId="5" r:id="rId3"/>
-    <sheet name="BFT" sheetId="4" r:id="rId4"/>
+    <sheet name="BFT" sheetId="4" r:id="rId1"/>
+    <sheet name="MDA" sheetId="2" r:id="rId2"/>
+    <sheet name="ICT" sheetId="6" r:id="rId3"/>
+    <sheet name="BST" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -211,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,30 +626,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -671,9 +647,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -691,6 +664,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1041,6 +1041,1476 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB20BDB5-1C3E-4612-867E-E135B5B8E9C9}">
+  <dimension ref="B2:AK30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
+    <col min="7" max="32" width="9.42578125" style="3" hidden="1" customWidth="1"/>
+    <col min="33" max="37" width="9.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+    </row>
+    <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6">
+        <v>3</v>
+      </c>
+      <c r="J3" s="6">
+        <v>4</v>
+      </c>
+      <c r="K3" s="6">
+        <v>5</v>
+      </c>
+      <c r="L3" s="6">
+        <v>6</v>
+      </c>
+      <c r="M3" s="6">
+        <v>7</v>
+      </c>
+      <c r="N3" s="6">
+        <v>8</v>
+      </c>
+      <c r="O3" s="6">
+        <v>9</v>
+      </c>
+      <c r="P3" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>11</v>
+      </c>
+      <c r="R3" s="6">
+        <v>12</v>
+      </c>
+      <c r="S3" s="6">
+        <v>13</v>
+      </c>
+      <c r="T3" s="6">
+        <v>14</v>
+      </c>
+      <c r="U3" s="6">
+        <v>15</v>
+      </c>
+      <c r="V3" s="6">
+        <v>16</v>
+      </c>
+      <c r="W3" s="6">
+        <v>17</v>
+      </c>
+      <c r="X3" s="6">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>19</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>20</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>21</v>
+      </c>
+      <c r="AB3" s="6">
+        <v>22</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>23</v>
+      </c>
+      <c r="AD3" s="6">
+        <v>24</v>
+      </c>
+      <c r="AE3" s="6">
+        <v>25</v>
+      </c>
+      <c r="AF3" s="6">
+        <v>26</v>
+      </c>
+      <c r="AG3" s="6">
+        <v>27</v>
+      </c>
+      <c r="AH3" s="6">
+        <v>28</v>
+      </c>
+      <c r="AI3" s="6">
+        <v>29</v>
+      </c>
+      <c r="AJ3" s="6">
+        <v>30</v>
+      </c>
+      <c r="AK3" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="11">
+        <v>0.94220000000000004</v>
+      </c>
+      <c r="AH4" s="11">
+        <v>0.93889999999999996</v>
+      </c>
+      <c r="AI4" s="10"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="13"/>
+    </row>
+    <row r="5" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B5" s="35"/>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>0.82609999999999995</v>
+      </c>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="14"/>
+    </row>
+    <row r="6" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B6" s="35"/>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="4">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="AH6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="14"/>
+    </row>
+    <row r="7" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B7" s="35"/>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="14"/>
+    </row>
+    <row r="8" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="14"/>
+    </row>
+    <row r="9" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="36"/>
+      <c r="C9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="18">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="15"/>
+      <c r="AJ9" s="15"/>
+      <c r="AK9" s="16"/>
+    </row>
+    <row r="10" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="10"/>
+      <c r="AK10" s="13"/>
+    </row>
+    <row r="11" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="14"/>
+    </row>
+    <row r="12" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="4">
+        <v>0.96</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="8">
+        <v>0.94972067039106145</v>
+      </c>
+      <c r="AH12" s="8">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="14"/>
+    </row>
+    <row r="13" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="8">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="AH13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="14"/>
+    </row>
+    <row r="14" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="14"/>
+    </row>
+    <row r="15" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="14"/>
+    </row>
+    <row r="16" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="8">
+        <v>0.93939393939393945</v>
+      </c>
+      <c r="AH16" s="8">
+        <v>0.84615384615384615</v>
+      </c>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="14"/>
+    </row>
+    <row r="17" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="14"/>
+    </row>
+    <row r="18" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B18" s="35"/>
+      <c r="C18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="14"/>
+    </row>
+    <row r="19" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B19" s="35"/>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH19" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="14"/>
+    </row>
+    <row r="20" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B20" s="37"/>
+      <c r="C20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH20" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
+      <c r="AK20" s="28"/>
+    </row>
+    <row r="21" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="19"/>
+      <c r="AE21" s="19"/>
+      <c r="AF21" s="19"/>
+      <c r="AG21" s="20">
+        <v>0.19839999999999999</v>
+      </c>
+      <c r="AH21" s="19"/>
+      <c r="AI21" s="19"/>
+      <c r="AJ21" s="19"/>
+      <c r="AK21" s="21"/>
+    </row>
+    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B22" s="30"/>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="8">
+        <v>0.81469999999999998</v>
+      </c>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="22"/>
+    </row>
+    <row r="23" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B23" s="30"/>
+      <c r="C23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="4">
+        <v>0.92820000000000003</v>
+      </c>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="22"/>
+    </row>
+    <row r="24" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B24" s="30"/>
+      <c r="C24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="22"/>
+    </row>
+    <row r="25" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B25" s="30"/>
+      <c r="C25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="22"/>
+    </row>
+    <row r="26" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B26" s="30"/>
+      <c r="C26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="22"/>
+    </row>
+    <row r="27" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B27" s="30"/>
+      <c r="C27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="2"/>
+      <c r="AK27" s="22"/>
+    </row>
+    <row r="28" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B28" s="30"/>
+      <c r="C28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="2"/>
+      <c r="AK28" s="22"/>
+    </row>
+    <row r="29" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B29" s="30"/>
+      <c r="C29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+      <c r="AJ29" s="2"/>
+      <c r="AK29" s="22"/>
+    </row>
+    <row r="30" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B30" s="31"/>
+      <c r="C30" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="23"/>
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
+      <c r="Y30" s="23"/>
+      <c r="Z30" s="23"/>
+      <c r="AA30" s="23"/>
+      <c r="AB30" s="23"/>
+      <c r="AC30" s="23"/>
+      <c r="AD30" s="23"/>
+      <c r="AE30" s="23"/>
+      <c r="AF30" s="23"/>
+      <c r="AG30" s="23"/>
+      <c r="AH30" s="23"/>
+      <c r="AI30" s="23"/>
+      <c r="AJ30" s="23"/>
+      <c r="AK30" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B21:B30"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:AK2"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B10:B20"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E10:E20"/>
+  </mergeCells>
+  <conditionalFormatting sqref="AG22">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"NP"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG10:AK20">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"NP"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;KFFFF00 Wiwynn Confidential</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B094723-5E1D-4BA3-A183-A6B78E7ACFF2}">
   <dimension ref="B2:AI27"/>
   <sheetViews>
@@ -1048,7 +2518,7 @@
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1057,54 +2527,54 @@
     <col min="5" max="35" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-    </row>
-    <row r="3" spans="2:35">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -1199,8 +2669,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:35">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B4" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1241,8 +2711,8 @@
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
     </row>
-    <row r="5" spans="2:35">
-      <c r="B5" s="19"/>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1281,8 +2751,8 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
     </row>
-    <row r="6" spans="2:35">
-      <c r="B6" s="19"/>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B6" s="32"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1321,8 +2791,8 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="2:35">
-      <c r="B7" s="19"/>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B7" s="32"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1361,8 +2831,8 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="8" spans="2:35">
-      <c r="B8" s="19"/>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1401,8 +2871,8 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="9" spans="2:35">
-      <c r="B9" s="19"/>
+    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1441,8 +2911,8 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
     </row>
-    <row r="10" spans="2:35">
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1481,8 +2951,8 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="2:35">
-      <c r="B11" s="19"/>
+    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1519,8 +2989,8 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="2:35">
-      <c r="B12" s="19"/>
+    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1557,8 +3027,8 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="2:35">
-      <c r="B13" s="19"/>
+    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B13" s="32"/>
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1595,8 +3065,8 @@
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="2:35">
-      <c r="B14" s="19"/>
+    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B14" s="32"/>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1633,8 +3103,8 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="2:35">
-      <c r="B15" s="19"/>
+    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1671,8 +3141,8 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="2:35">
-      <c r="B16" s="19"/>
+    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B16" s="32"/>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1709,8 +3179,8 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="2:35">
-      <c r="B17" s="19"/>
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B17" s="32"/>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1747,8 +3217,8 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="2:35">
-      <c r="B18" s="19"/>
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B18" s="32"/>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1785,8 +3255,8 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="2:35">
-      <c r="B19" s="19"/>
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B19" s="32"/>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1823,8 +3293,8 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="2:35">
-      <c r="B20" s="19" t="s">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B20" s="32" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1863,8 +3333,8 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="2:35">
-      <c r="B21" s="19"/>
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B21" s="32"/>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1901,8 +3371,8 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="2:35">
-      <c r="B22" s="19"/>
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1939,8 +3409,8 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="2:35">
-      <c r="B23" s="19"/>
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B23" s="32"/>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1977,8 +3447,8 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="2:35">
-      <c r="B24" s="19"/>
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B24" s="32"/>
       <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2015,8 +3485,8 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
     </row>
-    <row r="25" spans="2:35">
-      <c r="B25" s="19"/>
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B25" s="32"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
@@ -2053,8 +3523,8 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="2:35">
-      <c r="B26" s="19"/>
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B26" s="32"/>
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2091,8 +3561,8 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
     </row>
-    <row r="27" spans="2:35">
-      <c r="B27" s="19"/>
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B27" s="32"/>
       <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
@@ -2146,7 +3616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E74EE3C-55CD-4CB0-A9E9-4DB77100083E}">
   <dimension ref="B2:AI27"/>
   <sheetViews>
@@ -2154,7 +3624,7 @@
       <selection activeCell="C5" sqref="C5:C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -2163,54 +3633,54 @@
     <col min="5" max="35" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-    </row>
-    <row r="3" spans="2:35">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -2305,8 +3775,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:35">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B4" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2347,8 +3817,8 @@
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
     </row>
-    <row r="5" spans="2:35">
-      <c r="B5" s="19"/>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2387,8 +3857,8 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
     </row>
-    <row r="6" spans="2:35">
-      <c r="B6" s="19"/>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B6" s="32"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2427,8 +3897,8 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="2:35">
-      <c r="B7" s="19"/>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B7" s="32"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2467,8 +3937,8 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="8" spans="2:35">
-      <c r="B8" s="19"/>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2507,8 +3977,8 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="9" spans="2:35">
-      <c r="B9" s="19"/>
+    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2547,8 +4017,8 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
     </row>
-    <row r="10" spans="2:35">
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -2587,8 +4057,8 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="2:35">
-      <c r="B11" s="19"/>
+    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
@@ -2625,8 +4095,8 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="2:35">
-      <c r="B12" s="19"/>
+    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
@@ -2663,8 +4133,8 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="2:35">
-      <c r="B13" s="19"/>
+    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B13" s="32"/>
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
@@ -2701,8 +4171,8 @@
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="2:35">
-      <c r="B14" s="19"/>
+    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B14" s="32"/>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
@@ -2739,8 +4209,8 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="2:35">
-      <c r="B15" s="19"/>
+    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -2777,8 +4247,8 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="2:35">
-      <c r="B16" s="19"/>
+    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B16" s="32"/>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
@@ -2815,8 +4285,8 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="2:35">
-      <c r="B17" s="19"/>
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B17" s="32"/>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
@@ -2853,8 +4323,8 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="2:35">
-      <c r="B18" s="19"/>
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B18" s="32"/>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
@@ -2891,8 +4361,8 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="2:35">
-      <c r="B19" s="19"/>
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B19" s="32"/>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
@@ -2929,8 +4399,8 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="2:35">
-      <c r="B20" s="19" t="s">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B20" s="32" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -2969,8 +4439,8 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="2:35">
-      <c r="B21" s="19"/>
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B21" s="32"/>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
@@ -3007,8 +4477,8 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="2:35">
-      <c r="B22" s="19"/>
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
@@ -3045,8 +4515,8 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="2:35">
-      <c r="B23" s="19"/>
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B23" s="32"/>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
@@ -3083,8 +4553,8 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="2:35">
-      <c r="B24" s="19"/>
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B24" s="32"/>
       <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
@@ -3121,8 +4591,8 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
     </row>
-    <row r="25" spans="2:35">
-      <c r="B25" s="19"/>
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B25" s="32"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
@@ -3159,8 +4629,8 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="2:35">
-      <c r="B26" s="19"/>
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B26" s="32"/>
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
@@ -3197,8 +4667,8 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
     </row>
-    <row r="27" spans="2:35">
-      <c r="B27" s="19"/>
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B27" s="32"/>
       <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
@@ -3252,7 +4722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8839AD7D-30F6-41C7-84A2-68684993968A}">
   <dimension ref="B2:AI27"/>
   <sheetViews>
@@ -3261,7 +4731,7 @@
       <selection pane="topRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -3270,54 +4740,54 @@
     <col min="5" max="35" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-    </row>
-    <row r="3" spans="2:35">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -3412,8 +4882,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:35">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B4" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -3454,8 +4924,8 @@
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
     </row>
-    <row r="5" spans="2:35">
-      <c r="B5" s="19"/>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3494,8 +4964,8 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
     </row>
-    <row r="6" spans="2:35">
-      <c r="B6" s="19"/>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B6" s="32"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -3534,8 +5004,8 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="2:35">
-      <c r="B7" s="19"/>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B7" s="32"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -3574,8 +5044,8 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="8" spans="2:35">
-      <c r="B8" s="19"/>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -3614,8 +5084,8 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="9" spans="2:35">
-      <c r="B9" s="19"/>
+    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -3654,8 +5124,8 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
     </row>
-    <row r="10" spans="2:35" hidden="1">
-      <c r="B10" s="19" t="s">
+    <row r="10" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -3694,8 +5164,8 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="2:35" hidden="1">
-      <c r="B11" s="19"/>
+    <row r="11" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
@@ -3732,8 +5202,8 @@
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="2:35" hidden="1">
-      <c r="B12" s="19"/>
+    <row r="12" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="32"/>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
@@ -3770,8 +5240,8 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="2:35" hidden="1">
-      <c r="B13" s="19"/>
+    <row r="13" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="32"/>
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
@@ -3808,8 +5278,8 @@
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="2:35" hidden="1">
-      <c r="B14" s="19"/>
+    <row r="14" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="32"/>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
@@ -3846,8 +5316,8 @@
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="2:35" hidden="1">
-      <c r="B15" s="19"/>
+    <row r="15" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -3884,8 +5354,8 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="2:35" hidden="1">
-      <c r="B16" s="19"/>
+    <row r="16" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="32"/>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
@@ -3922,8 +5392,8 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="2:35" hidden="1">
-      <c r="B17" s="19"/>
+    <row r="17" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="32"/>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
@@ -3960,8 +5430,8 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="2:35" hidden="1">
-      <c r="B18" s="19"/>
+    <row r="18" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="32"/>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3998,8 +5468,8 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="2:35" hidden="1">
-      <c r="B19" s="19"/>
+    <row r="19" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="32"/>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
@@ -4036,8 +5506,8 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
     </row>
-    <row r="20" spans="2:35" hidden="1">
-      <c r="B20" s="19" t="s">
+    <row r="20" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="32" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -4076,8 +5546,8 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
     </row>
-    <row r="21" spans="2:35" hidden="1">
-      <c r="B21" s="19"/>
+    <row r="21" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="32"/>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
@@ -4114,8 +5584,8 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="2:35" hidden="1">
-      <c r="B22" s="19"/>
+    <row r="22" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
@@ -4152,8 +5622,8 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="2:35" hidden="1">
-      <c r="B23" s="19"/>
+    <row r="23" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="32"/>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
@@ -4190,8 +5660,8 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
     </row>
-    <row r="24" spans="2:35" hidden="1">
-      <c r="B24" s="19"/>
+    <row r="24" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="32"/>
       <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
@@ -4228,8 +5698,8 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
     </row>
-    <row r="25" spans="2:35" hidden="1">
-      <c r="B25" s="19"/>
+    <row r="25" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="32"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
@@ -4266,8 +5736,8 @@
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
     </row>
-    <row r="26" spans="2:35" hidden="1">
-      <c r="B26" s="19"/>
+    <row r="26" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="32"/>
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
@@ -4304,8 +5774,8 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
     </row>
-    <row r="27" spans="2:35" hidden="1">
-      <c r="B27" s="19"/>
+    <row r="27" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="32"/>
       <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
@@ -4352,1476 +5822,6 @@
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="B10:B19"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;KFFFF00 Wiwynn Confidential</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB20BDB5-1C3E-4612-867E-E135B5B8E9C9}">
-  <dimension ref="B2:AK30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH23" sqref="AH23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
-    <col min="7" max="32" width="9.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="33" max="37" width="9.42578125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:37" ht="14.45">
-      <c r="B2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-    </row>
-    <row r="3" spans="2:37" thickBot="1">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="6">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6">
-        <v>2</v>
-      </c>
-      <c r="I3" s="6">
-        <v>3</v>
-      </c>
-      <c r="J3" s="6">
-        <v>4</v>
-      </c>
-      <c r="K3" s="6">
-        <v>5</v>
-      </c>
-      <c r="L3" s="6">
-        <v>6</v>
-      </c>
-      <c r="M3" s="6">
-        <v>7</v>
-      </c>
-      <c r="N3" s="6">
-        <v>8</v>
-      </c>
-      <c r="O3" s="6">
-        <v>9</v>
-      </c>
-      <c r="P3" s="6">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>11</v>
-      </c>
-      <c r="R3" s="6">
-        <v>12</v>
-      </c>
-      <c r="S3" s="6">
-        <v>13</v>
-      </c>
-      <c r="T3" s="6">
-        <v>14</v>
-      </c>
-      <c r="U3" s="6">
-        <v>15</v>
-      </c>
-      <c r="V3" s="6">
-        <v>16</v>
-      </c>
-      <c r="W3" s="6">
-        <v>17</v>
-      </c>
-      <c r="X3" s="6">
-        <v>18</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>19</v>
-      </c>
-      <c r="Z3" s="6">
-        <v>20</v>
-      </c>
-      <c r="AA3" s="6">
-        <v>21</v>
-      </c>
-      <c r="AB3" s="6">
-        <v>22</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>23</v>
-      </c>
-      <c r="AD3" s="6">
-        <v>24</v>
-      </c>
-      <c r="AE3" s="6">
-        <v>25</v>
-      </c>
-      <c r="AF3" s="6">
-        <v>26</v>
-      </c>
-      <c r="AG3" s="6">
-        <v>27</v>
-      </c>
-      <c r="AH3" s="6">
-        <v>28</v>
-      </c>
-      <c r="AI3" s="6">
-        <v>29</v>
-      </c>
-      <c r="AJ3" s="6">
-        <v>30</v>
-      </c>
-      <c r="AK3" s="6">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="2:37" ht="14.45">
-      <c r="B4" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11">
-        <v>0.95</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="11">
-        <v>0.94220000000000004</v>
-      </c>
-      <c r="AH4" s="11">
-        <v>0.93889999999999996</v>
-      </c>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="13"/>
-    </row>
-    <row r="5" spans="2:37" ht="14.45">
-      <c r="B5" s="21"/>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2"/>
-      <c r="AG5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="4">
-        <v>0.82609999999999995</v>
-      </c>
-      <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="14"/>
-    </row>
-    <row r="6" spans="2:37" ht="14.45">
-      <c r="B6" s="21"/>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="4">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="AH6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="14"/>
-    </row>
-    <row r="7" spans="2:37" ht="14.45">
-      <c r="B7" s="21"/>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="14"/>
-    </row>
-    <row r="8" spans="2:37" ht="14.45">
-      <c r="B8" s="21"/>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI8" s="2"/>
-      <c r="AJ8" s="2"/>
-      <c r="AK8" s="14"/>
-    </row>
-    <row r="9" spans="2:37" thickBot="1">
-      <c r="B9" s="22"/>
-      <c r="C9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="17">
-        <v>0.95</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="15"/>
-      <c r="AE9" s="15"/>
-      <c r="AF9" s="15"/>
-      <c r="AG9" s="18">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="18">
-        <v>1</v>
-      </c>
-      <c r="AI9" s="15"/>
-      <c r="AJ9" s="15"/>
-      <c r="AK9" s="16"/>
-    </row>
-    <row r="10" spans="2:37" ht="14.45">
-      <c r="B10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0.95</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="13"/>
-    </row>
-    <row r="11" spans="2:37" ht="14.45">
-      <c r="B11" s="21"/>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
-      <c r="AK11" s="14"/>
-    </row>
-    <row r="12" spans="2:37" ht="14.45">
-      <c r="B12" s="21"/>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="4">
-        <v>0.96</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="2"/>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="8">
-        <v>0.94972067039106145</v>
-      </c>
-      <c r="AH12" s="8">
-        <v>0.36363636363636365</v>
-      </c>
-      <c r="AI12" s="2"/>
-      <c r="AJ12" s="2"/>
-      <c r="AK12" s="14"/>
-    </row>
-    <row r="13" spans="2:37" ht="14.45">
-      <c r="B13" s="21"/>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AG13" s="8">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="AH13" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="14"/>
-    </row>
-    <row r="14" spans="2:37" ht="14.45">
-      <c r="B14" s="21"/>
-      <c r="C14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI14" s="2"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="14"/>
-    </row>
-    <row r="15" spans="2:37" ht="14.45">
-      <c r="B15" s="21"/>
-      <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI15" s="2"/>
-      <c r="AJ15" s="2"/>
-      <c r="AK15" s="14"/>
-    </row>
-    <row r="16" spans="2:37" ht="14.45">
-      <c r="B16" s="21"/>
-      <c r="C16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="2"/>
-      <c r="AG16" s="8">
-        <v>0.93939393939393945</v>
-      </c>
-      <c r="AH16" s="8">
-        <v>0.84615384615384615</v>
-      </c>
-      <c r="AI16" s="2"/>
-      <c r="AJ16" s="2"/>
-      <c r="AK16" s="14"/>
-    </row>
-    <row r="17" spans="2:37" ht="14.45">
-      <c r="B17" s="21"/>
-      <c r="C17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="14"/>
-    </row>
-    <row r="18" spans="2:37" ht="14.45">
-      <c r="B18" s="21"/>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="2"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="14"/>
-    </row>
-    <row r="19" spans="2:37">
-      <c r="B19" s="21"/>
-      <c r="C19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="2"/>
-      <c r="AD19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="2"/>
-      <c r="AG19" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH19" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI19" s="2"/>
-      <c r="AJ19" s="2"/>
-      <c r="AK19" s="14"/>
-    </row>
-    <row r="20" spans="2:37">
-      <c r="B20" s="34"/>
-      <c r="C20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6"/>
-      <c r="AE20" s="6"/>
-      <c r="AF20" s="6"/>
-      <c r="AG20" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH20" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI20" s="6"/>
-      <c r="AJ20" s="6"/>
-      <c r="AK20" s="37"/>
-    </row>
-    <row r="21" spans="2:37">
-      <c r="B21" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="28">
-        <v>0.95</v>
-      </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="27"/>
-      <c r="Z21" s="27"/>
-      <c r="AA21" s="27"/>
-      <c r="AB21" s="27"/>
-      <c r="AC21" s="27"/>
-      <c r="AD21" s="27"/>
-      <c r="AE21" s="27"/>
-      <c r="AF21" s="27"/>
-      <c r="AG21" s="28">
-        <v>0.19839999999999999</v>
-      </c>
-      <c r="AH21" s="27"/>
-      <c r="AI21" s="27"/>
-      <c r="AJ21" s="27"/>
-      <c r="AK21" s="29"/>
-    </row>
-    <row r="22" spans="2:37">
-      <c r="B22" s="39"/>
-      <c r="C22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="2"/>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="2"/>
-      <c r="AD22" s="2"/>
-      <c r="AE22" s="2"/>
-      <c r="AF22" s="2"/>
-      <c r="AG22" s="8">
-        <v>0.81469999999999998</v>
-      </c>
-      <c r="AH22" s="2"/>
-      <c r="AI22" s="2"/>
-      <c r="AJ22" s="2"/>
-      <c r="AK22" s="30"/>
-    </row>
-    <row r="23" spans="2:37">
-      <c r="B23" s="39"/>
-      <c r="C23" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="2"/>
-      <c r="Z23" s="2"/>
-      <c r="AA23" s="2"/>
-      <c r="AB23" s="2"/>
-      <c r="AC23" s="2"/>
-      <c r="AD23" s="2"/>
-      <c r="AE23" s="2"/>
-      <c r="AF23" s="2"/>
-      <c r="AG23" s="4">
-        <v>0.92820000000000003</v>
-      </c>
-      <c r="AH23" s="2"/>
-      <c r="AI23" s="2"/>
-      <c r="AJ23" s="2"/>
-      <c r="AK23" s="30"/>
-    </row>
-    <row r="24" spans="2:37">
-      <c r="B24" s="39"/>
-      <c r="C24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
-      <c r="Z24" s="2"/>
-      <c r="AA24" s="2"/>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="2"/>
-      <c r="AD24" s="2"/>
-      <c r="AE24" s="2"/>
-      <c r="AF24" s="2"/>
-      <c r="AG24" s="2"/>
-      <c r="AH24" s="2"/>
-      <c r="AI24" s="2"/>
-      <c r="AJ24" s="2"/>
-      <c r="AK24" s="30"/>
-    </row>
-    <row r="25" spans="2:37">
-      <c r="B25" s="39"/>
-      <c r="C25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="2"/>
-      <c r="AA25" s="2"/>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="2"/>
-      <c r="AD25" s="2"/>
-      <c r="AE25" s="2"/>
-      <c r="AF25" s="2"/>
-      <c r="AG25" s="2"/>
-      <c r="AH25" s="2"/>
-      <c r="AI25" s="2"/>
-      <c r="AJ25" s="2"/>
-      <c r="AK25" s="30"/>
-    </row>
-    <row r="26" spans="2:37">
-      <c r="B26" s="39"/>
-      <c r="C26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="X26" s="2"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="2"/>
-      <c r="AA26" s="2"/>
-      <c r="AB26" s="2"/>
-      <c r="AC26" s="2"/>
-      <c r="AD26" s="2"/>
-      <c r="AE26" s="2"/>
-      <c r="AF26" s="2"/>
-      <c r="AG26" s="2"/>
-      <c r="AH26" s="2"/>
-      <c r="AI26" s="2"/>
-      <c r="AJ26" s="2"/>
-      <c r="AK26" s="30"/>
-    </row>
-    <row r="27" spans="2:37">
-      <c r="B27" s="39"/>
-      <c r="C27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="2"/>
-      <c r="AA27" s="2"/>
-      <c r="AB27" s="2"/>
-      <c r="AC27" s="2"/>
-      <c r="AD27" s="2"/>
-      <c r="AE27" s="2"/>
-      <c r="AF27" s="2"/>
-      <c r="AG27" s="2"/>
-      <c r="AH27" s="2"/>
-      <c r="AI27" s="2"/>
-      <c r="AJ27" s="2"/>
-      <c r="AK27" s="30"/>
-    </row>
-    <row r="28" spans="2:37">
-      <c r="B28" s="39"/>
-      <c r="C28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-      <c r="X28" s="2"/>
-      <c r="Y28" s="2"/>
-      <c r="Z28" s="2"/>
-      <c r="AA28" s="2"/>
-      <c r="AB28" s="2"/>
-      <c r="AC28" s="2"/>
-      <c r="AD28" s="2"/>
-      <c r="AE28" s="2"/>
-      <c r="AF28" s="2"/>
-      <c r="AG28" s="2"/>
-      <c r="AH28" s="2"/>
-      <c r="AI28" s="2"/>
-      <c r="AJ28" s="2"/>
-      <c r="AK28" s="30"/>
-    </row>
-    <row r="29" spans="2:37">
-      <c r="B29" s="39"/>
-      <c r="C29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="2"/>
-      <c r="AA29" s="2"/>
-      <c r="AB29" s="2"/>
-      <c r="AC29" s="2"/>
-      <c r="AD29" s="2"/>
-      <c r="AE29" s="2"/>
-      <c r="AF29" s="2"/>
-      <c r="AG29" s="2"/>
-      <c r="AH29" s="2"/>
-      <c r="AI29" s="2"/>
-      <c r="AJ29" s="2"/>
-      <c r="AK29" s="30"/>
-    </row>
-    <row r="30" spans="2:37">
-      <c r="B30" s="40"/>
-      <c r="C30" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="32">
-        <v>0.95</v>
-      </c>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="31"/>
-      <c r="R30" s="31"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="31"/>
-      <c r="U30" s="31"/>
-      <c r="V30" s="31"/>
-      <c r="W30" s="31"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="31"/>
-      <c r="Z30" s="31"/>
-      <c r="AA30" s="31"/>
-      <c r="AB30" s="31"/>
-      <c r="AC30" s="31"/>
-      <c r="AD30" s="31"/>
-      <c r="AE30" s="31"/>
-      <c r="AF30" s="31"/>
-      <c r="AG30" s="31"/>
-      <c r="AH30" s="31"/>
-      <c r="AI30" s="31"/>
-      <c r="AJ30" s="31"/>
-      <c r="AK30" s="33"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:AK2"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B10:B20"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E10:E20"/>
-    <mergeCell ref="B21:B30"/>
-  </mergeCells>
-  <conditionalFormatting sqref="AG10:AK20">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"NP"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"NP"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;KFFFF00 Wiwynn Confidential</oddFooter>
@@ -6051,13 +6051,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C61952FF-CFDA-4B33-87EE-300359AA6E33}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C61952FF-CFDA-4B33-87EE-300359AA6E33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D576C1-94E9-4F34-97F4-B0F7A0DC703A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D576C1-94E9-4F34-97F4-B0F7A0DC703A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="727bea6f-0c2a-4892-b5ab-62a21362c92d"/>
+    <ds:schemaRef ds:uri="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{523FC5AD-E615-4897-BF95-CF120637FEEB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{523FC5AD-E615-4897-BF95-CF120637FEEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
+    <ds:schemaRef ds:uri="727bea6f-0c2a-4892-b5ab-62a21362c92d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
modified:   Engineering Yield Tracker (1).xlsx 	modified:   app.py
</commit_message>
<xml_diff>
--- a/Engineering Yield Tracker (1).xlsx
+++ b/Engineering Yield Tracker (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudadmwiwynn-my.sharepoint.com/personal/syahirah_sabudin_wiwynn_com/Documents/Documents/Umi/FPY-monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B256F41-77E7-4439-8567-3F0F32F2D32B}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{286D10D8-0EFF-4113-AE7E-EDA3B17FC7D4}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12585" xr2:uid="{FA83E918-ED32-4BA0-A84E-C85110B79042}"/>
   </bookViews>
@@ -1044,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB20BDB5-1C3E-4612-867E-E135B5B8E9C9}">
   <dimension ref="B2:AK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5830,26 +5830,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="727bea6f-0c2a-4892-b5ab-62a21362c92d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="886a63ba-0744-4b0b-a434-895fa6fc36ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003232E4788D58D14183140D27ED20215A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e7b2bbbc29d0f10e8a3f78354e64a9e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="886a63ba-0744-4b0b-a434-895fa6fc36ce" xmlns:ns3="727bea6f-0c2a-4892-b5ab-62a21362c92d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f56b1e5d1cff782aeb72e4afee55e13" ns2:_="" ns3:_="">
     <xsd:import namespace="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
@@ -6050,10 +6030,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="727bea6f-0c2a-4892-b5ab-62a21362c92d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="886a63ba-0744-4b0b-a434-895fa6fc36ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C61952FF-CFDA-4B33-87EE-300359AA6E33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{523FC5AD-E615-4897-BF95-CF120637FEEB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
+    <ds:schemaRef ds:uri="727bea6f-0c2a-4892-b5ab-62a21362c92d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6070,20 +6081,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{523FC5AD-E615-4897-BF95-CF120637FEEB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C61952FF-CFDA-4B33-87EE-300359AA6E33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
-    <ds:schemaRef ds:uri="727bea6f-0c2a-4892-b5ab-62a21362c92d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
modified:   Engineering Yield Tracker (1).xlsx 	modified:   FPY-dashboard.html 	modified:   app.py 	modified:   templates/index.html
</commit_message>
<xml_diff>
--- a/Engineering Yield Tracker (1).xlsx
+++ b/Engineering Yield Tracker (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudadmwiwynn-my.sharepoint.com/personal/syahirah_sabudin_wiwynn_com/Documents/Documents/Umi/FPY-monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{286D10D8-0EFF-4113-AE7E-EDA3B17FC7D4}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{532C294E-CCC0-4090-9345-44C637CB86A3}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12585" xr2:uid="{FA83E918-ED32-4BA0-A84E-C85110B79042}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12585" xr2:uid="{FA83E918-ED32-4BA0-A84E-C85110B79042}"/>
   </bookViews>
   <sheets>
     <sheet name="BFT" sheetId="4" r:id="rId1"/>
@@ -1045,7 +1045,7 @@
   <dimension ref="B2:AK30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,8 +1056,7 @@
     <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
-    <col min="7" max="32" width="9.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="33" max="37" width="9.42578125" style="3" customWidth="1"/>
+    <col min="7" max="37" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:37" x14ac:dyDescent="0.25">
@@ -5830,6 +5829,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="727bea6f-0c2a-4892-b5ab-62a21362c92d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="886a63ba-0744-4b0b-a434-895fa6fc36ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003232E4788D58D14183140D27ED20215A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e7b2bbbc29d0f10e8a3f78354e64a9e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="886a63ba-0744-4b0b-a434-895fa6fc36ce" xmlns:ns3="727bea6f-0c2a-4892-b5ab-62a21362c92d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f56b1e5d1cff782aeb72e4afee55e13" ns2:_="" ns3:_="">
     <xsd:import namespace="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
@@ -6030,27 +6049,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="727bea6f-0c2a-4892-b5ab-62a21362c92d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="886a63ba-0744-4b0b-a434-895fa6fc36ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C61952FF-CFDA-4B33-87EE-300359AA6E33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D576C1-94E9-4F34-97F4-B0F7A0DC703A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="727bea6f-0c2a-4892-b5ab-62a21362c92d"/>
+    <ds:schemaRef ds:uri="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{523FC5AD-E615-4897-BF95-CF120637FEEB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6067,23 +6085,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D576C1-94E9-4F34-97F4-B0F7A0DC703A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="727bea6f-0c2a-4892-b5ab-62a21362c92d"/>
-    <ds:schemaRef ds:uri="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C61952FF-CFDA-4B33-87EE-300359AA6E33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
modified:   Engineering Yield Tracker (1).xlsx
</commit_message>
<xml_diff>
--- a/Engineering Yield Tracker (1).xlsx
+++ b/Engineering Yield Tracker (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudadmwiwynn-my.sharepoint.com/personal/syahirah_sabudin_wiwynn_com/Documents/Documents/Umi/FPY-monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1467443-A8EB-462B-80CE-160E5AA2ABF7}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F592BCAB-9629-4D77-B4F4-EF123CC49F1C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{FA83E918-ED32-4BA0-A84E-C85110B79042}"/>
   </bookViews>
@@ -570,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -653,6 +653,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -688,15 +700,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1050,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB20BDB5-1C3E-4612-867E-E135B5B8E9C9}">
   <dimension ref="B2:AK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AO20" sqref="AO20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,68 +1063,67 @@
     <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
-    <col min="7" max="32" width="9.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="33" max="37" width="9.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="37" width="9.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="31"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="32"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="6">
         <v>1</v>
       </c>
@@ -1217,7 +1219,7 @@
       </c>
     </row>
     <row r="4" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -1230,14 +1232,30 @@
       <c r="F4" s="11">
         <v>0.95</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="G4" s="11">
+        <v>0.9798</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.98350000000000004</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.99229999999999996</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.98780000000000001</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="L4" s="10">
+        <v>99.21</v>
+      </c>
+      <c r="M4" s="31">
+        <v>1</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0.98909999999999998</v>
+      </c>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
@@ -1268,12 +1286,12 @@
       <c r="AJ4" s="11">
         <v>0.94530000000000003</v>
       </c>
-      <c r="AK4" s="40">
+      <c r="AK4" s="28">
         <v>0.99019999999999997</v>
       </c>
     </row>
     <row r="5" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1322,12 +1340,12 @@
       <c r="AJ5" s="4">
         <v>0.93110000000000004</v>
       </c>
-      <c r="AK5" s="41">
+      <c r="AK5" s="29">
         <v>0.98480000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1376,12 +1394,12 @@
       <c r="AJ6" s="4">
         <v>0.93559999999999999</v>
       </c>
-      <c r="AK6" s="41">
+      <c r="AK6" s="29">
         <v>0.92779999999999996</v>
       </c>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1430,12 +1448,12 @@
       <c r="AJ7" s="4">
         <v>0.95020000000000004</v>
       </c>
-      <c r="AK7" s="41">
+      <c r="AK7" s="29">
         <v>0.9456</v>
       </c>
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1484,12 +1502,12 @@
       <c r="AJ8" s="4">
         <v>0.97099999999999997</v>
       </c>
-      <c r="AK8" s="41">
+      <c r="AK8" s="29">
         <v>0.95650000000000002</v>
       </c>
     </row>
     <row r="9" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
@@ -1538,12 +1556,12 @@
       <c r="AJ9" s="16">
         <v>0.94669999999999999</v>
       </c>
-      <c r="AK9" s="42">
+      <c r="AK9" s="30">
         <v>0.97760000000000002</v>
       </c>
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1552,7 +1570,7 @@
       <c r="D10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="42" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="11">
@@ -1595,14 +1613,14 @@
       <c r="AK10" s="13"/>
     </row>
     <row r="11" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B11" s="34"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="4">
         <v>0.95</v>
       </c>
@@ -1643,14 +1661,14 @@
       <c r="AK11" s="14"/>
     </row>
     <row r="12" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="4">
         <v>0.96</v>
       </c>
@@ -1691,14 +1709,14 @@
       <c r="AK12" s="14"/>
     </row>
     <row r="13" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="9" t="s">
         <v>42</v>
       </c>
@@ -1739,14 +1757,14 @@
       <c r="AK13" s="14"/>
     </row>
     <row r="14" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B14" s="34"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="43"/>
       <c r="F14" s="9" t="s">
         <v>42</v>
       </c>
@@ -1787,14 +1805,14 @@
       <c r="AK14" s="14"/>
     </row>
     <row r="15" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="9" t="s">
         <v>42</v>
       </c>
@@ -1835,14 +1853,14 @@
       <c r="AK15" s="14"/>
     </row>
     <row r="16" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="9" t="s">
         <v>42</v>
       </c>
@@ -1883,14 +1901,14 @@
       <c r="AK16" s="14"/>
     </row>
     <row r="17" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="9" t="s">
         <v>42</v>
       </c>
@@ -1931,14 +1949,14 @@
       <c r="AK17" s="14"/>
     </row>
     <row r="18" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="39"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="9" t="s">
         <v>42</v>
       </c>
@@ -1979,14 +1997,14 @@
       <c r="AK18" s="14"/>
     </row>
     <row r="19" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="39"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="9" t="s">
         <v>42</v>
       </c>
@@ -2027,14 +2045,14 @@
       <c r="AK19" s="14"/>
     </row>
     <row r="20" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B20" s="36"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="25" t="s">
         <v>42</v>
       </c>
@@ -2075,7 +2093,7 @@
       <c r="AK20" s="27"/>
     </row>
     <row r="21" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="32" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -2123,7 +2141,7 @@
       <c r="AK21" s="20"/>
     </row>
     <row r="22" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B22" s="29"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
@@ -2169,7 +2187,7 @@
       <c r="AK22" s="21"/>
     </row>
     <row r="23" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B23" s="29"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="2" t="s">
         <v>47</v>
       </c>
@@ -2215,7 +2233,7 @@
       <c r="AK23" s="21"/>
     </row>
     <row r="24" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B24" s="29"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="2" t="s">
         <v>48</v>
       </c>
@@ -2259,7 +2277,7 @@
       <c r="AK24" s="21"/>
     </row>
     <row r="25" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B25" s="29"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="2" t="s">
         <v>26</v>
       </c>
@@ -2303,7 +2321,7 @@
       <c r="AK25" s="21"/>
     </row>
     <row r="26" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B26" s="29"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
@@ -2347,7 +2365,7 @@
       <c r="AK26" s="21"/>
     </row>
     <row r="27" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B27" s="29"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
@@ -2391,7 +2409,7 @@
       <c r="AK27" s="21"/>
     </row>
     <row r="28" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B28" s="29"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="2" t="s">
         <v>51</v>
       </c>
@@ -2435,7 +2453,7 @@
       <c r="AK28" s="21"/>
     </row>
     <row r="29" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B29" s="29"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="2" t="s">
         <v>52</v>
       </c>
@@ -2479,7 +2497,7 @@
       <c r="AK29" s="21"/>
     </row>
     <row r="30" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B30" s="30"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="22" t="s">
         <v>53</v>
       </c>
@@ -2570,53 +2588,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
     </row>
     <row r="3" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -2712,7 +2730,7 @@
       </c>
     </row>
     <row r="4" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2754,7 +2772,7 @@
       <c r="AI4" s="2"/>
     </row>
     <row r="5" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B5" s="31"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2794,7 +2812,7 @@
       <c r="AI5" s="2"/>
     </row>
     <row r="6" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2834,7 +2852,7 @@
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2874,7 +2892,7 @@
       <c r="AI7" s="2"/>
     </row>
     <row r="8" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2914,7 +2932,7 @@
       <c r="AI8" s="2"/>
     </row>
     <row r="9" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2954,7 +2972,7 @@
       <c r="AI9" s="2"/>
     </row>
     <row r="10" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -2994,7 +3012,7 @@
       <c r="AI10" s="2"/>
     </row>
     <row r="11" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
@@ -3032,7 +3050,7 @@
       <c r="AI11" s="2"/>
     </row>
     <row r="12" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
@@ -3070,7 +3088,7 @@
       <c r="AI12" s="2"/>
     </row>
     <row r="13" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
@@ -3108,7 +3126,7 @@
       <c r="AI13" s="2"/>
     </row>
     <row r="14" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
@@ -3146,7 +3164,7 @@
       <c r="AI14" s="2"/>
     </row>
     <row r="15" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B15" s="31"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -3184,7 +3202,7 @@
       <c r="AI15" s="2"/>
     </row>
     <row r="16" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
@@ -3222,7 +3240,7 @@
       <c r="AI16" s="2"/>
     </row>
     <row r="17" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
@@ -3260,7 +3278,7 @@
       <c r="AI17" s="2"/>
     </row>
     <row r="18" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3298,7 +3316,7 @@
       <c r="AI18" s="2"/>
     </row>
     <row r="19" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3336,7 +3354,7 @@
       <c r="AI19" s="2"/>
     </row>
     <row r="20" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="35" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -3376,7 +3394,7 @@
       <c r="AI20" s="2"/>
     </row>
     <row r="21" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
@@ -3414,7 +3432,7 @@
       <c r="AI21" s="2"/>
     </row>
     <row r="22" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B22" s="31"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
@@ -3452,7 +3470,7 @@
       <c r="AI22" s="2"/>
     </row>
     <row r="23" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
@@ -3490,7 +3508,7 @@
       <c r="AI23" s="2"/>
     </row>
     <row r="24" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
@@ -3528,7 +3546,7 @@
       <c r="AI24" s="2"/>
     </row>
     <row r="25" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
@@ -3566,7 +3584,7 @@
       <c r="AI25" s="2"/>
     </row>
     <row r="26" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
@@ -3604,7 +3622,7 @@
       <c r="AI26" s="2"/>
     </row>
     <row r="27" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
@@ -3676,53 +3694,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
     </row>
     <row r="3" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -3818,7 +3836,7 @@
       </c>
     </row>
     <row r="4" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -3860,7 +3878,7 @@
       <c r="AI4" s="2"/>
     </row>
     <row r="5" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B5" s="31"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3900,7 +3918,7 @@
       <c r="AI5" s="2"/>
     </row>
     <row r="6" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -3940,7 +3958,7 @@
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -3980,7 +3998,7 @@
       <c r="AI7" s="2"/>
     </row>
     <row r="8" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -4020,7 +4038,7 @@
       <c r="AI8" s="2"/>
     </row>
     <row r="9" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -4060,7 +4078,7 @@
       <c r="AI9" s="2"/>
     </row>
     <row r="10" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -4100,7 +4118,7 @@
       <c r="AI10" s="2"/>
     </row>
     <row r="11" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
@@ -4138,7 +4156,7 @@
       <c r="AI11" s="2"/>
     </row>
     <row r="12" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
@@ -4176,7 +4194,7 @@
       <c r="AI12" s="2"/>
     </row>
     <row r="13" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
@@ -4214,7 +4232,7 @@
       <c r="AI13" s="2"/>
     </row>
     <row r="14" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
@@ -4252,7 +4270,7 @@
       <c r="AI14" s="2"/>
     </row>
     <row r="15" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B15" s="31"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -4290,7 +4308,7 @@
       <c r="AI15" s="2"/>
     </row>
     <row r="16" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
@@ -4328,7 +4346,7 @@
       <c r="AI16" s="2"/>
     </row>
     <row r="17" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
@@ -4366,7 +4384,7 @@
       <c r="AI17" s="2"/>
     </row>
     <row r="18" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
@@ -4404,7 +4422,7 @@
       <c r="AI18" s="2"/>
     </row>
     <row r="19" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
@@ -4442,7 +4460,7 @@
       <c r="AI19" s="2"/>
     </row>
     <row r="20" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="35" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -4482,7 +4500,7 @@
       <c r="AI20" s="2"/>
     </row>
     <row r="21" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
@@ -4520,7 +4538,7 @@
       <c r="AI21" s="2"/>
     </row>
     <row r="22" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B22" s="31"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
@@ -4558,7 +4576,7 @@
       <c r="AI22" s="2"/>
     </row>
     <row r="23" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
@@ -4596,7 +4614,7 @@
       <c r="AI23" s="2"/>
     </row>
     <row r="24" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
@@ -4634,7 +4652,7 @@
       <c r="AI24" s="2"/>
     </row>
     <row r="25" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
@@ -4672,7 +4690,7 @@
       <c r="AI25" s="2"/>
     </row>
     <row r="26" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
@@ -4710,7 +4728,7 @@
       <c r="AI26" s="2"/>
     </row>
     <row r="27" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
@@ -4783,53 +4801,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
     </row>
     <row r="3" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
       <c r="E3" s="2">
         <v>1</v>
       </c>
@@ -4925,7 +4943,7 @@
       </c>
     </row>
     <row r="4" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -4967,7 +4985,7 @@
       <c r="AI4" s="2"/>
     </row>
     <row r="5" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B5" s="31"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -5007,7 +5025,7 @@
       <c r="AI5" s="2"/>
     </row>
     <row r="6" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -5047,7 +5065,7 @@
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -5087,7 +5105,7 @@
       <c r="AI7" s="2"/>
     </row>
     <row r="8" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -5127,7 +5145,7 @@
       <c r="AI8" s="2"/>
     </row>
     <row r="9" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -5167,7 +5185,7 @@
       <c r="AI9" s="2"/>
     </row>
     <row r="10" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -5207,7 +5225,7 @@
       <c r="AI10" s="2"/>
     </row>
     <row r="11" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
@@ -5245,7 +5263,7 @@
       <c r="AI11" s="2"/>
     </row>
     <row r="12" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
@@ -5283,7 +5301,7 @@
       <c r="AI12" s="2"/>
     </row>
     <row r="13" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
@@ -5321,7 +5339,7 @@
       <c r="AI13" s="2"/>
     </row>
     <row r="14" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
@@ -5359,7 +5377,7 @@
       <c r="AI14" s="2"/>
     </row>
     <row r="15" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
@@ -5397,7 +5415,7 @@
       <c r="AI15" s="2"/>
     </row>
     <row r="16" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
@@ -5435,7 +5453,7 @@
       <c r="AI16" s="2"/>
     </row>
     <row r="17" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
@@ -5473,7 +5491,7 @@
       <c r="AI17" s="2"/>
     </row>
     <row r="18" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
@@ -5511,7 +5529,7 @@
       <c r="AI18" s="2"/>
     </row>
     <row r="19" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
@@ -5549,7 +5567,7 @@
       <c r="AI19" s="2"/>
     </row>
     <row r="20" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="35" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -5589,7 +5607,7 @@
       <c r="AI20" s="2"/>
     </row>
     <row r="21" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
@@ -5627,7 +5645,7 @@
       <c r="AI21" s="2"/>
     </row>
     <row r="22" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="31"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
@@ -5665,7 +5683,7 @@
       <c r="AI22" s="2"/>
     </row>
     <row r="23" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
@@ -5703,7 +5721,7 @@
       <c r="AI23" s="2"/>
     </row>
     <row r="24" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
@@ -5741,7 +5759,7 @@
       <c r="AI24" s="2"/>
     </row>
     <row r="25" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
@@ -5779,7 +5797,7 @@
       <c r="AI25" s="2"/>
     </row>
     <row r="26" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
@@ -5817,7 +5835,7 @@
       <c r="AI26" s="2"/>
     </row>
     <row r="27" spans="2:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
new file:   dummy data import.py
</commit_message>
<xml_diff>
--- a/Engineering Yield Tracker (1).xlsx
+++ b/Engineering Yield Tracker (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cloudadmwiwynn-my.sharepoint.com/personal/syahirah_sabudin_wiwynn_com/Documents/Documents/Umi/FPY-monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F592BCAB-9629-4D77-B4F4-EF123CC49F1C}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="13_ncr:1_{6582128B-6ACA-427D-9255-E10632809678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8818EC56-B8F3-4685-A931-F58FC02A41E8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{FA83E918-ED32-4BA0-A84E-C85110B79042}"/>
+    <workbookView minimized="1" xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="12585" xr2:uid="{FA83E918-ED32-4BA0-A84E-C85110B79042}"/>
   </bookViews>
   <sheets>
     <sheet name="BFT" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="53">
   <si>
     <t>Customer</t>
   </si>
@@ -166,9 +166,6 @@
 However, the FPY value here is for reference only. 
 Actual might different from MIC ATE Report, 
 Because had checked with HQ MTE Will, daily Input and daily retest in shopfloor will take non-fresh board into the count (For Fiona project)</t>
-  </si>
-  <si>
-    <t>NP</t>
   </si>
   <si>
     <t>TBC</t>
@@ -1054,7 +1051,7 @@
   <dimension ref="B2:AK30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,8 +1244,8 @@
       <c r="K4" s="11">
         <v>0.99670000000000003</v>
       </c>
-      <c r="L4" s="10">
-        <v>99.21</v>
+      <c r="L4" s="11">
+        <v>0.99209999999999998</v>
       </c>
       <c r="M4" s="31">
         <v>1</v>
@@ -1256,8 +1253,12 @@
       <c r="N4" s="11">
         <v>0.98909999999999998</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="11">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="P4" s="11">
+        <v>0.97929999999999995</v>
+      </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
@@ -1274,21 +1275,11 @@
       <c r="AD4" s="10"/>
       <c r="AE4" s="10"/>
       <c r="AF4" s="10"/>
-      <c r="AG4" s="11">
-        <v>0.94220000000000004</v>
-      </c>
-      <c r="AH4" s="11">
-        <v>0.93889999999999996</v>
-      </c>
-      <c r="AI4" s="11">
-        <v>0.94369999999999998</v>
-      </c>
-      <c r="AJ4" s="11">
-        <v>0.94530000000000003</v>
-      </c>
-      <c r="AK4" s="28">
-        <v>0.99019999999999997</v>
-      </c>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="28"/>
     </row>
     <row r="5" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B5" s="38"/>
@@ -1328,21 +1319,11 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
-      <c r="AG5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="4">
-        <v>0.82609999999999995</v>
-      </c>
-      <c r="AI5" s="4">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="AJ5" s="4">
-        <v>0.93110000000000004</v>
-      </c>
-      <c r="AK5" s="29">
-        <v>0.98480000000000001</v>
-      </c>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="29"/>
     </row>
     <row r="6" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B6" s="38"/>
@@ -1382,21 +1363,11 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
-      <c r="AG6" s="4">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="AH6" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="4">
-        <v>0.96779999999999999</v>
-      </c>
-      <c r="AJ6" s="4">
-        <v>0.93559999999999999</v>
-      </c>
-      <c r="AK6" s="29">
-        <v>0.92779999999999996</v>
-      </c>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="29"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B7" s="38"/>
@@ -1436,21 +1407,11 @@
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
-      <c r="AG7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="4">
-        <v>0.95450000000000002</v>
-      </c>
-      <c r="AJ7" s="4">
-        <v>0.95020000000000004</v>
-      </c>
-      <c r="AK7" s="29">
-        <v>0.9456</v>
-      </c>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="29"/>
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B8" s="38"/>
@@ -1490,21 +1451,11 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
-      <c r="AG8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI8" s="4">
-        <v>0.98209999999999997</v>
-      </c>
-      <c r="AJ8" s="4">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="AK8" s="29">
-        <v>0.95650000000000002</v>
-      </c>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="29"/>
     </row>
     <row r="9" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="39"/>
@@ -1544,21 +1495,11 @@
       <c r="AD9" s="15"/>
       <c r="AE9" s="15"/>
       <c r="AF9" s="15"/>
-      <c r="AG9" s="17">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="17">
-        <v>1</v>
-      </c>
-      <c r="AI9" s="16">
-        <v>0.92430000000000001</v>
-      </c>
-      <c r="AJ9" s="16">
-        <v>0.94669999999999999</v>
-      </c>
-      <c r="AK9" s="30">
-        <v>0.97760000000000002</v>
-      </c>
+      <c r="AG9" s="17"/>
+      <c r="AH9" s="17"/>
+      <c r="AI9" s="16"/>
+      <c r="AJ9" s="16"/>
+      <c r="AK9" s="30"/>
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B10" s="37" t="s">
@@ -1602,12 +1543,8 @@
       <c r="AD10" s="10"/>
       <c r="AE10" s="10"/>
       <c r="AF10" s="10"/>
-      <c r="AG10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH10" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
       <c r="AI10" s="10"/>
       <c r="AJ10" s="10"/>
       <c r="AK10" s="13"/>
@@ -1650,12 +1587,8 @@
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
-      <c r="AG11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH11" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
       <c r="AK11" s="14"/>
@@ -1698,12 +1631,8 @@
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
-      <c r="AG12" s="8">
-        <v>0.94972067039106145</v>
-      </c>
-      <c r="AH12" s="8">
-        <v>0.36363636363636365</v>
-      </c>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="14"/>
@@ -1718,7 +1647,7 @@
       </c>
       <c r="E13" s="43"/>
       <c r="F13" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1746,12 +1675,8 @@
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
-      <c r="AG13" s="8">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="AH13" s="8">
-        <v>1</v>
-      </c>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
       <c r="AI13" s="2"/>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="14"/>
@@ -1759,14 +1684,14 @@
     <row r="14" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B14" s="38"/>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="43"/>
       <c r="F14" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1794,12 +1719,8 @@
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
-      <c r="AG14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH14" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="14"/>
@@ -1807,14 +1728,14 @@
     <row r="15" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B15" s="38"/>
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="43"/>
       <c r="F15" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1842,12 +1763,8 @@
       <c r="AD15" s="2"/>
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
-      <c r="AG15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH15" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="AG15" s="8"/>
+      <c r="AH15" s="8"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
       <c r="AK15" s="14"/>
@@ -1862,7 +1779,7 @@
       </c>
       <c r="E16" s="43"/>
       <c r="F16" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1890,12 +1807,8 @@
       <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
-      <c r="AG16" s="8">
-        <v>0.93939393939393945</v>
-      </c>
-      <c r="AH16" s="8">
-        <v>0.84615384615384615</v>
-      </c>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
       <c r="AK16" s="14"/>
@@ -1910,7 +1823,7 @@
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1938,12 +1851,8 @@
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
-      <c r="AG17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH17" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
       <c r="AK17" s="14"/>
@@ -1958,7 +1867,7 @@
       </c>
       <c r="E18" s="43"/>
       <c r="F18" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1986,12 +1895,8 @@
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
-      <c r="AG18" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="8"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
       <c r="AK18" s="14"/>
@@ -1999,14 +1904,14 @@
     <row r="19" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B19" s="38"/>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="43"/>
       <c r="F19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -2034,12 +1939,8 @@
       <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
-      <c r="AG19" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH19" s="8">
-        <v>1</v>
-      </c>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
       <c r="AK19" s="14"/>
@@ -2054,7 +1955,7 @@
       </c>
       <c r="E20" s="43"/>
       <c r="F20" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -2082,12 +1983,8 @@
       <c r="AD20" s="6"/>
       <c r="AE20" s="6"/>
       <c r="AF20" s="6"/>
-      <c r="AG20" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH20" s="26" t="s">
-        <v>41</v>
-      </c>
+      <c r="AG20" s="26"/>
+      <c r="AH20" s="26"/>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="6"/>
       <c r="AK20" s="27"/>
@@ -2100,7 +1997,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="19">
@@ -2132,9 +2029,7 @@
       <c r="AD21" s="18"/>
       <c r="AE21" s="18"/>
       <c r="AF21" s="18"/>
-      <c r="AG21" s="19">
-        <v>0.19839999999999999</v>
-      </c>
+      <c r="AG21" s="19"/>
       <c r="AH21" s="18"/>
       <c r="AI21" s="18"/>
       <c r="AJ21" s="18"/>
@@ -2146,7 +2041,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="4">
@@ -2178,9 +2073,7 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
       <c r="AF22" s="2"/>
-      <c r="AG22" s="8">
-        <v>0.81469999999999998</v>
-      </c>
+      <c r="AG22" s="8"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="2"/>
@@ -2189,10 +2082,10 @@
     <row r="23" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="4">
@@ -2224,9 +2117,7 @@
       <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
-      <c r="AG23" s="4">
-        <v>0.92820000000000003</v>
-      </c>
+      <c r="AG23" s="4"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
@@ -2235,10 +2126,10 @@
     <row r="24" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="4">
@@ -2282,7 +2173,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="4">
@@ -2326,7 +2217,7 @@
         <v>27</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="4">
@@ -2370,7 +2261,7 @@
         <v>28</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="4">
@@ -2411,10 +2302,10 @@
     <row r="28" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B28" s="33"/>
       <c r="C28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="4">
@@ -2455,10 +2346,10 @@
     <row r="29" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B29" s="33"/>
       <c r="C29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="4">
@@ -2499,10 +2390,10 @@
     <row r="30" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B30" s="34"/>
       <c r="C30" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="23">
@@ -5890,6 +5781,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="727bea6f-0c2a-4892-b5ab-62a21362c92d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="886a63ba-0744-4b0b-a434-895fa6fc36ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003232E4788D58D14183140D27ED20215A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e7b2bbbc29d0f10e8a3f78354e64a9e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="886a63ba-0744-4b0b-a434-895fa6fc36ce" xmlns:ns3="727bea6f-0c2a-4892-b5ab-62a21362c92d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f56b1e5d1cff782aeb72e4afee55e13" ns2:_="" ns3:_="">
     <xsd:import namespace="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
@@ -6090,27 +6001,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="727bea6f-0c2a-4892-b5ab-62a21362c92d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="886a63ba-0744-4b0b-a434-895fa6fc36ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C61952FF-CFDA-4B33-87EE-300359AA6E33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D576C1-94E9-4F34-97F4-B0F7A0DC703A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="727bea6f-0c2a-4892-b5ab-62a21362c92d"/>
+    <ds:schemaRef ds:uri="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{523FC5AD-E615-4897-BF95-CF120637FEEB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6127,23 +6037,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D576C1-94E9-4F34-97F4-B0F7A0DC703A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="727bea6f-0c2a-4892-b5ab-62a21362c92d"/>
-    <ds:schemaRef ds:uri="886a63ba-0744-4b0b-a434-895fa6fc36ce"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C61952FF-CFDA-4B33-87EE-300359AA6E33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>